<commit_message>
Improved layout of dynamic topic model and geocoding
</commit_message>
<xml_diff>
--- a/output/tables/topic_terms.xlsx
+++ b/output/tables/topic_terms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AmericanRevolution\revolution\output\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6A69EE43-7945-4C48-9438-161A69175B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45237A61-7928-44C9-9588-AF93ADE8D586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topic_terms" sheetId="1" r:id="rId1"/>
@@ -364,9 +364,6 @@
     <t>heart</t>
   </si>
   <si>
-    <t>Ã </t>
-  </si>
-  <si>
     <t>road</t>
   </si>
   <si>
@@ -898,9 +895,6 @@
     <t>gun</t>
   </si>
   <si>
-    <t>quâ€™il</t>
-  </si>
-  <si>
     <t>satisfaction</t>
   </si>
   <si>
@@ -1505,12 +1499,18 @@
   </si>
   <si>
     <t>mon</t>
+  </si>
+  <si>
+    <t>quant</t>
+  </si>
+  <si>
+    <t>la</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2365,10 +2365,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2773,57 +2775,57 @@
         <v>113</v>
       </c>
       <c r="AB4" t="s">
+        <v>494</v>
+      </c>
+      <c r="AC4" t="s">
         <v>114</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>115</v>
       </c>
       <c r="AD4" t="s">
         <v>72</v>
       </c>
       <c r="AE4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
         <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" t="s">
         <v>43</v>
       </c>
       <c r="E5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" t="s">
         <v>119</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>120</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>121</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>122</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>123</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>124</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>125</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>126</v>
-      </c>
-      <c r="M5" t="s">
-        <v>127</v>
       </c>
       <c r="N5" t="s">
         <v>112</v>
@@ -2832,10 +2834,10 @@
         <v>60</v>
       </c>
       <c r="P5" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q5" t="s">
         <v>128</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>129</v>
       </c>
       <c r="R5" t="s">
         <v>77</v>
@@ -2844,176 +2846,176 @@
         <v>72</v>
       </c>
       <c r="T5" t="s">
+        <v>129</v>
+      </c>
+      <c r="U5" t="s">
+        <v>117</v>
+      </c>
+      <c r="V5" t="s">
         <v>130</v>
-      </c>
-      <c r="U5" t="s">
-        <v>118</v>
-      </c>
-      <c r="V5" t="s">
-        <v>131</v>
       </c>
       <c r="W5" t="s">
         <v>47</v>
       </c>
       <c r="X5" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y5" t="s">
         <v>132</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>133</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB5" t="s">
         <v>134</v>
       </c>
-      <c r="AA5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>135</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>136</v>
       </c>
       <c r="AD5" t="s">
         <v>48</v>
       </c>
       <c r="AE5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
       </c>
       <c r="C6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" t="s">
         <v>139</v>
-      </c>
-      <c r="D6" t="s">
-        <v>140</v>
       </c>
       <c r="E6" t="s">
         <v>49</v>
       </c>
       <c r="F6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" t="s">
         <v>141</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>142</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>143</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>144</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>145</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>146</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>147</v>
       </c>
-      <c r="M6" t="s">
-        <v>148</v>
-      </c>
       <c r="N6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O6" t="s">
         <v>77</v>
       </c>
       <c r="P6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q6" t="s">
+        <v>148</v>
+      </c>
+      <c r="R6" t="s">
         <v>149</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>150</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>151</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>152</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>153</v>
-      </c>
-      <c r="V6" t="s">
-        <v>154</v>
       </c>
       <c r="W6" t="s">
         <v>91</v>
       </c>
       <c r="X6" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y6" t="s">
         <v>155</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>156</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>157</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>158</v>
       </c>
       <c r="AB6" t="s">
         <v>84</v>
       </c>
       <c r="AC6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AD6" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE6" t="s">
         <v>159</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" t="s">
         <v>161</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>162</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>163</v>
-      </c>
-      <c r="D7" t="s">
-        <v>164</v>
       </c>
       <c r="E7" t="s">
         <v>60</v>
       </c>
       <c r="F7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" t="s">
         <v>165</v>
-      </c>
-      <c r="G7" t="s">
-        <v>166</v>
       </c>
       <c r="H7" t="s">
         <v>44</v>
       </c>
       <c r="I7" t="s">
+        <v>166</v>
+      </c>
+      <c r="J7" t="s">
         <v>167</v>
-      </c>
-      <c r="J7" t="s">
-        <v>168</v>
       </c>
       <c r="K7" t="s">
         <v>60</v>
       </c>
       <c r="L7" t="s">
+        <v>168</v>
+      </c>
+      <c r="M7" t="s">
         <v>169</v>
-      </c>
-      <c r="M7" t="s">
-        <v>170</v>
       </c>
       <c r="N7" t="s">
         <v>38</v>
@@ -3028,43 +3030,43 @@
         <v>86</v>
       </c>
       <c r="R7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S7" t="s">
         <v>70</v>
       </c>
       <c r="T7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="U7" t="s">
         <v>36</v>
       </c>
       <c r="V7" t="s">
+        <v>172</v>
+      </c>
+      <c r="W7" t="s">
         <v>173</v>
-      </c>
-      <c r="W7" t="s">
-        <v>174</v>
       </c>
       <c r="X7" t="s">
         <v>60</v>
       </c>
       <c r="Y7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Z7" t="s">
         <v>95</v>
       </c>
       <c r="AA7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB7" t="s">
         <v>176</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>177</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>178</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>179</v>
       </c>
       <c r="AE7" t="s">
         <v>47</v>
@@ -3072,25 +3074,25 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8" t="s">
         <v>108</v>
       </c>
       <c r="C8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" t="s">
         <v>181</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" t="s">
         <v>182</v>
       </c>
-      <c r="E8" t="s">
-        <v>125</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>183</v>
-      </c>
-      <c r="G8" t="s">
-        <v>184</v>
       </c>
       <c r="H8" t="s">
         <v>45</v>
@@ -3105,61 +3107,61 @@
         <v>87</v>
       </c>
       <c r="L8" t="s">
+        <v>184</v>
+      </c>
+      <c r="M8" t="s">
+        <v>129</v>
+      </c>
+      <c r="N8" t="s">
         <v>185</v>
-      </c>
-      <c r="M8" t="s">
-        <v>130</v>
-      </c>
-      <c r="N8" t="s">
-        <v>186</v>
       </c>
       <c r="O8" t="s">
         <v>41</v>
       </c>
       <c r="P8" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q8" t="s">
         <v>187</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
+        <v>178</v>
+      </c>
+      <c r="S8" t="s">
         <v>188</v>
       </c>
-      <c r="R8" t="s">
-        <v>179</v>
-      </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>189</v>
-      </c>
-      <c r="T8" t="s">
-        <v>190</v>
       </c>
       <c r="U8" t="s">
         <v>60</v>
       </c>
       <c r="V8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="W8" t="s">
+        <v>190</v>
+      </c>
+      <c r="X8" t="s">
         <v>191</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>192</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>193</v>
       </c>
       <c r="Z8" t="s">
         <v>43</v>
       </c>
       <c r="AA8" t="s">
+        <v>193</v>
+      </c>
+      <c r="AB8" t="s">
         <v>194</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AD8" t="s">
         <v>195</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>132</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>196</v>
       </c>
       <c r="AE8" t="s">
         <v>46</v>
@@ -3167,91 +3169,91 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" t="s">
         <v>197</v>
-      </c>
-      <c r="B9" t="s">
-        <v>198</v>
       </c>
       <c r="C9" t="s">
         <v>53</v>
       </c>
       <c r="D9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" t="s">
         <v>199</v>
-      </c>
-      <c r="E9" t="s">
-        <v>200</v>
       </c>
       <c r="F9" t="s">
         <v>49</v>
       </c>
       <c r="G9" t="s">
+        <v>200</v>
+      </c>
+      <c r="H9" t="s">
         <v>201</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>202</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>203</v>
-      </c>
-      <c r="J9" t="s">
-        <v>204</v>
       </c>
       <c r="K9" t="s">
         <v>31</v>
       </c>
       <c r="L9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N9" t="s">
         <v>47</v>
       </c>
       <c r="O9" t="s">
+        <v>205</v>
+      </c>
+      <c r="P9" t="s">
         <v>206</v>
       </c>
-      <c r="P9" t="s">
-        <v>207</v>
-      </c>
       <c r="Q9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="R9" t="s">
         <v>41</v>
       </c>
       <c r="S9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="T9" t="s">
         <v>56</v>
       </c>
       <c r="U9" t="s">
+        <v>207</v>
+      </c>
+      <c r="V9" t="s">
         <v>208</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>209</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>210</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>211</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>212</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>213</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>214</v>
       </c>
-      <c r="AB9" t="s">
-        <v>215</v>
-      </c>
       <c r="AC9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AD9" t="s">
         <v>92</v>
@@ -3262,52 +3264,52 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B10" t="s">
         <v>216</v>
-      </c>
-      <c r="B10" t="s">
-        <v>217</v>
       </c>
       <c r="C10" t="s">
         <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E10" t="s">
+        <v>217</v>
+      </c>
+      <c r="F10" t="s">
         <v>218</v>
-      </c>
-      <c r="F10" t="s">
-        <v>219</v>
       </c>
       <c r="G10" t="s">
         <v>96</v>
       </c>
       <c r="H10" t="s">
+        <v>219</v>
+      </c>
+      <c r="I10" t="s">
         <v>220</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>221</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>222</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>223</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>224</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>225</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>226</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>227</v>
-      </c>
-      <c r="P10" t="s">
-        <v>228</v>
       </c>
       <c r="Q10" t="s">
         <v>46</v>
@@ -3316,233 +3318,233 @@
         <v>72</v>
       </c>
       <c r="S10" t="s">
+        <v>228</v>
+      </c>
+      <c r="T10" t="s">
         <v>229</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
+        <v>197</v>
+      </c>
+      <c r="V10" t="s">
         <v>230</v>
       </c>
-      <c r="U10" t="s">
-        <v>198</v>
-      </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>231</v>
       </c>
-      <c r="W10" t="s">
-        <v>232</v>
-      </c>
       <c r="X10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Y10" t="s">
         <v>72</v>
       </c>
       <c r="Z10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AA10" t="s">
         <v>110</v>
       </c>
       <c r="AB10" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>189</v>
+      </c>
+      <c r="AD10" t="s">
         <v>233</v>
       </c>
-      <c r="AC10" t="s">
-        <v>190</v>
-      </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>234</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D11" t="s">
         <v>72</v>
       </c>
       <c r="E11" t="s">
+        <v>236</v>
+      </c>
+      <c r="F11" t="s">
         <v>237</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>238</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>239</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" t="s">
         <v>240</v>
-      </c>
-      <c r="I11" t="s">
-        <v>118</v>
-      </c>
-      <c r="J11" t="s">
-        <v>241</v>
       </c>
       <c r="K11" t="s">
         <v>43</v>
       </c>
       <c r="L11" t="s">
+        <v>241</v>
+      </c>
+      <c r="M11" t="s">
         <v>242</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>243</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>244</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q11" t="s">
         <v>245</v>
       </c>
-      <c r="P11" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>246</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>247</v>
       </c>
-      <c r="S11" t="s">
-        <v>248</v>
-      </c>
       <c r="T11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="U11" t="s">
         <v>47</v>
       </c>
       <c r="V11" t="s">
+        <v>248</v>
+      </c>
+      <c r="W11" t="s">
         <v>249</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>250</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>225</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB11" t="s">
         <v>251</v>
       </c>
-      <c r="Y11" t="s">
-        <v>116</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>226</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>132</v>
-      </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>252</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE11" t="s">
         <v>253</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>138</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12" t="s">
         <v>255</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>256</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" t="s">
         <v>257</v>
-      </c>
-      <c r="D12" t="s">
-        <v>167</v>
-      </c>
-      <c r="E12" t="s">
-        <v>258</v>
       </c>
       <c r="F12" t="s">
         <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H12" t="s">
         <v>77</v>
       </c>
       <c r="I12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J12" t="s">
+        <v>259</v>
+      </c>
+      <c r="K12" t="s">
         <v>260</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>261</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>262</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>263</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>264</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>265</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>266</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>267</v>
       </c>
       <c r="R12" t="s">
         <v>106</v>
       </c>
       <c r="S12" t="s">
+        <v>267</v>
+      </c>
+      <c r="T12" t="s">
         <v>268</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>269</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>270</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>271</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>272</v>
-      </c>
-      <c r="X12" t="s">
-        <v>273</v>
       </c>
       <c r="Y12" t="s">
         <v>96</v>
       </c>
       <c r="Z12" t="s">
+        <v>273</v>
+      </c>
+      <c r="AA12" t="s">
         <v>274</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AB12" t="s">
         <v>275</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>276</v>
       </c>
       <c r="AC12" t="s">
         <v>60</v>
       </c>
       <c r="AD12" t="s">
+        <v>276</v>
+      </c>
+      <c r="AE12" t="s">
         <v>277</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -3550,76 +3552,76 @@
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C13" t="s">
         <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F13" t="s">
+        <v>279</v>
+      </c>
+      <c r="G13" t="s">
         <v>280</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>281</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" t="s">
         <v>282</v>
       </c>
-      <c r="I13" t="s">
-        <v>150</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>283</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>284</v>
-      </c>
-      <c r="L13" t="s">
-        <v>285</v>
       </c>
       <c r="M13" t="s">
         <v>60</v>
       </c>
       <c r="N13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P13" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q13" t="s">
         <v>286</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
+        <v>145</v>
+      </c>
+      <c r="S13" t="s">
+        <v>139</v>
+      </c>
+      <c r="T13" t="s">
         <v>287</v>
       </c>
-      <c r="R13" t="s">
-        <v>146</v>
-      </c>
-      <c r="S13" t="s">
-        <v>140</v>
-      </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>288</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>289</v>
       </c>
-      <c r="V13" t="s">
+      <c r="W13" t="s">
         <v>290</v>
       </c>
-      <c r="W13" t="s">
-        <v>291</v>
-      </c>
       <c r="X13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Y13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Z13" t="s">
         <v>96</v>
@@ -3628,60 +3630,60 @@
         <v>87</v>
       </c>
       <c r="AB13" t="s">
+        <v>493</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>291</v>
+      </c>
+      <c r="AE13" t="s">
         <v>292</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>192</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>293</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E14" t="s">
         <v>79</v>
       </c>
       <c r="F14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G14" t="s">
+        <v>296</v>
+      </c>
+      <c r="H14" t="s">
+        <v>297</v>
+      </c>
+      <c r="I14" t="s">
         <v>298</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J14" t="s">
+        <v>148</v>
+      </c>
+      <c r="K14" t="s">
         <v>299</v>
       </c>
-      <c r="I14" t="s">
+      <c r="L14" t="s">
         <v>300</v>
       </c>
-      <c r="J14" t="s">
-        <v>149</v>
-      </c>
-      <c r="K14" t="s">
-        <v>301</v>
-      </c>
-      <c r="L14" t="s">
-        <v>302</v>
-      </c>
       <c r="M14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O14" t="s">
         <v>89</v>
@@ -3693,46 +3695,46 @@
         <v>97</v>
       </c>
       <c r="R14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S14" t="s">
         <v>99</v>
       </c>
       <c r="T14" t="s">
+        <v>301</v>
+      </c>
+      <c r="U14" t="s">
+        <v>302</v>
+      </c>
+      <c r="V14" t="s">
         <v>303</v>
       </c>
-      <c r="U14" t="s">
+      <c r="W14" t="s">
         <v>304</v>
       </c>
-      <c r="V14" t="s">
+      <c r="X14" t="s">
         <v>305</v>
-      </c>
-      <c r="W14" t="s">
-        <v>306</v>
-      </c>
-      <c r="X14" t="s">
-        <v>307</v>
       </c>
       <c r="Y14" t="s">
         <v>38</v>
       </c>
       <c r="Z14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="AA14" t="s">
         <v>84</v>
       </c>
       <c r="AB14" t="s">
+        <v>307</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>305</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>308</v>
+      </c>
+      <c r="AE14" t="s">
         <v>309</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>307</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>310</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -3740,114 +3742,114 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C15" t="s">
         <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H15" t="s">
         <v>99</v>
       </c>
       <c r="I15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J15" t="s">
         <v>93</v>
       </c>
       <c r="K15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L15" t="s">
+        <v>312</v>
+      </c>
+      <c r="M15" t="s">
+        <v>313</v>
+      </c>
+      <c r="N15" t="s">
         <v>314</v>
       </c>
-      <c r="M15" t="s">
+      <c r="O15" t="s">
         <v>315</v>
       </c>
-      <c r="N15" t="s">
+      <c r="P15" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>221</v>
+      </c>
+      <c r="R15" t="s">
         <v>316</v>
       </c>
-      <c r="O15" t="s">
+      <c r="S15" t="s">
         <v>317</v>
       </c>
-      <c r="P15" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>222</v>
-      </c>
-      <c r="R15" t="s">
+      <c r="T15" t="s">
         <v>318</v>
       </c>
-      <c r="S15" t="s">
+      <c r="U15" t="s">
         <v>319</v>
       </c>
-      <c r="T15" t="s">
-        <v>320</v>
-      </c>
-      <c r="U15" t="s">
-        <v>321</v>
-      </c>
       <c r="V15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="W15" t="s">
         <v>46</v>
       </c>
       <c r="X15" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="Y15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Z15" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AA15" t="s">
         <v>54</v>
       </c>
       <c r="AB15" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AC15" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD15" t="s">
         <v>84</v>
       </c>
       <c r="AE15" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B16" t="s">
         <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D16" t="s">
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G16" t="s">
         <v>72</v>
@@ -3865,111 +3867,111 @@
         <v>86</v>
       </c>
       <c r="L16" t="s">
+        <v>328</v>
+      </c>
+      <c r="M16" t="s">
+        <v>329</v>
+      </c>
+      <c r="N16" t="s">
         <v>330</v>
       </c>
-      <c r="M16" t="s">
+      <c r="O16" t="s">
         <v>331</v>
       </c>
-      <c r="N16" t="s">
+      <c r="P16" t="s">
         <v>332</v>
       </c>
-      <c r="O16" t="s">
+      <c r="Q16" t="s">
         <v>333</v>
       </c>
-      <c r="P16" t="s">
+      <c r="R16" t="s">
         <v>334</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="S16" t="s">
         <v>335</v>
       </c>
-      <c r="R16" t="s">
-        <v>336</v>
-      </c>
-      <c r="S16" t="s">
-        <v>337</v>
-      </c>
       <c r="T16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U16" t="s">
         <v>48</v>
       </c>
       <c r="V16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="W16" t="s">
         <v>65</v>
       </c>
       <c r="X16" t="s">
+        <v>337</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>338</v>
+      </c>
+      <c r="AB16" t="s">
         <v>339</v>
       </c>
-      <c r="Y16" t="s">
-        <v>150</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>197</v>
-      </c>
-      <c r="AA16" t="s">
+      <c r="AC16" t="s">
         <v>340</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AD16" t="s">
+        <v>334</v>
+      </c>
+      <c r="AE16" t="s">
         <v>341</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>342</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>336</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F17" t="s">
+        <v>343</v>
+      </c>
+      <c r="G17" t="s">
+        <v>344</v>
+      </c>
+      <c r="H17" t="s">
+        <v>115</v>
+      </c>
+      <c r="I17" t="s">
         <v>345</v>
       </c>
-      <c r="G17" t="s">
+      <c r="J17" t="s">
+        <v>206</v>
+      </c>
+      <c r="K17" t="s">
+        <v>191</v>
+      </c>
+      <c r="L17" t="s">
         <v>346</v>
       </c>
-      <c r="H17" t="s">
-        <v>116</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="M17" t="s">
         <v>347</v>
       </c>
-      <c r="J17" t="s">
-        <v>207</v>
-      </c>
-      <c r="K17" t="s">
-        <v>192</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>348</v>
       </c>
-      <c r="M17" t="s">
+      <c r="O17" t="s">
         <v>349</v>
-      </c>
-      <c r="N17" t="s">
-        <v>350</v>
-      </c>
-      <c r="O17" t="s">
-        <v>351</v>
       </c>
       <c r="P17" t="s">
         <v>43</v>
@@ -3978,93 +3980,93 @@
         <v>90</v>
       </c>
       <c r="R17" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="S17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T17" t="s">
         <v>42</v>
       </c>
       <c r="U17" t="s">
+        <v>351</v>
+      </c>
+      <c r="V17" t="s">
+        <v>352</v>
+      </c>
+      <c r="W17" t="s">
+        <v>252</v>
+      </c>
+      <c r="X17" t="s">
         <v>353</v>
       </c>
-      <c r="V17" t="s">
+      <c r="Y17" t="s">
+        <v>283</v>
+      </c>
+      <c r="Z17" t="s">
         <v>354</v>
       </c>
-      <c r="W17" t="s">
-        <v>253</v>
-      </c>
-      <c r="X17" t="s">
+      <c r="AA17" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB17" t="s">
         <v>355</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>284</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>356</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>357</v>
       </c>
       <c r="AC17" t="s">
         <v>87</v>
       </c>
       <c r="AD17" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="AE17" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B18" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C18" t="s">
         <v>104</v>
       </c>
       <c r="D18" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E18" t="s">
         <v>72</v>
       </c>
       <c r="F18" t="s">
+        <v>360</v>
+      </c>
+      <c r="G18" t="s">
+        <v>257</v>
+      </c>
+      <c r="H18" t="s">
+        <v>361</v>
+      </c>
+      <c r="I18" t="s">
         <v>362</v>
       </c>
-      <c r="G18" t="s">
-        <v>258</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
+        <v>222</v>
+      </c>
+      <c r="K18" t="s">
+        <v>148</v>
+      </c>
+      <c r="L18" t="s">
         <v>363</v>
       </c>
-      <c r="I18" t="s">
+      <c r="M18" t="s">
         <v>364</v>
       </c>
-      <c r="J18" t="s">
-        <v>223</v>
-      </c>
-      <c r="K18" t="s">
-        <v>149</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
         <v>365</v>
       </c>
-      <c r="M18" t="s">
-        <v>366</v>
-      </c>
-      <c r="N18" t="s">
-        <v>367</v>
-      </c>
       <c r="O18" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="P18" t="s">
         <v>76</v>
@@ -4073,37 +4075,37 @@
         <v>65</v>
       </c>
       <c r="R18" t="s">
+        <v>366</v>
+      </c>
+      <c r="S18" t="s">
+        <v>367</v>
+      </c>
+      <c r="T18" t="s">
         <v>368</v>
       </c>
-      <c r="S18" t="s">
+      <c r="U18" t="s">
         <v>369</v>
       </c>
-      <c r="T18" t="s">
+      <c r="V18" t="s">
         <v>370</v>
       </c>
-      <c r="U18" t="s">
+      <c r="W18" t="s">
+        <v>289</v>
+      </c>
+      <c r="X18" t="s">
         <v>371</v>
       </c>
-      <c r="V18" t="s">
+      <c r="Y18" t="s">
         <v>372</v>
       </c>
-      <c r="W18" t="s">
-        <v>290</v>
-      </c>
-      <c r="X18" t="s">
+      <c r="Z18" t="s">
         <v>373</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="AA18" t="s">
         <v>374</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AB18" t="s">
         <v>375</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>376</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>377</v>
       </c>
       <c r="AC18" t="s">
         <v>38</v>
@@ -4112,173 +4114,173 @@
         <v>36</v>
       </c>
       <c r="AE18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B19" t="s">
+        <v>377</v>
+      </c>
+      <c r="C19" t="s">
+        <v>293</v>
+      </c>
+      <c r="D19" t="s">
+        <v>334</v>
+      </c>
+      <c r="E19" t="s">
+        <v>378</v>
+      </c>
+      <c r="F19" t="s">
         <v>379</v>
-      </c>
-      <c r="C19" t="s">
-        <v>295</v>
-      </c>
-      <c r="D19" t="s">
-        <v>336</v>
-      </c>
-      <c r="E19" t="s">
-        <v>380</v>
-      </c>
-      <c r="F19" t="s">
-        <v>381</v>
       </c>
       <c r="G19" t="s">
         <v>60</v>
       </c>
       <c r="H19" t="s">
+        <v>380</v>
+      </c>
+      <c r="I19" t="s">
+        <v>381</v>
+      </c>
+      <c r="J19" t="s">
+        <v>209</v>
+      </c>
+      <c r="K19" t="s">
+        <v>233</v>
+      </c>
+      <c r="L19" t="s">
         <v>382</v>
       </c>
-      <c r="I19" t="s">
+      <c r="M19" t="s">
         <v>383</v>
-      </c>
-      <c r="J19" t="s">
-        <v>210</v>
-      </c>
-      <c r="K19" t="s">
-        <v>234</v>
-      </c>
-      <c r="L19" t="s">
-        <v>384</v>
-      </c>
-      <c r="M19" t="s">
-        <v>385</v>
       </c>
       <c r="N19" t="s">
         <v>41</v>
       </c>
       <c r="O19" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="P19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Q19" t="s">
         <v>103</v>
       </c>
       <c r="R19" t="s">
+        <v>385</v>
+      </c>
+      <c r="S19" t="s">
+        <v>386</v>
+      </c>
+      <c r="T19" t="s">
         <v>387</v>
       </c>
-      <c r="S19" t="s">
+      <c r="U19" t="s">
+        <v>224</v>
+      </c>
+      <c r="V19" t="s">
+        <v>257</v>
+      </c>
+      <c r="W19" t="s">
         <v>388</v>
       </c>
-      <c r="T19" t="s">
+      <c r="X19" t="s">
         <v>389</v>
       </c>
-      <c r="U19" t="s">
-        <v>225</v>
-      </c>
-      <c r="V19" t="s">
-        <v>258</v>
-      </c>
-      <c r="W19" t="s">
+      <c r="Y19" t="s">
         <v>390</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Z19" t="s">
+        <v>263</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>272</v>
+      </c>
+      <c r="AB19" t="s">
         <v>391</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="AC19" t="s">
         <v>392</v>
       </c>
-      <c r="Z19" t="s">
-        <v>264</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>273</v>
-      </c>
-      <c r="AB19" t="s">
+      <c r="AD19" t="s">
         <v>393</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AE19" t="s">
         <v>394</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>395</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>395</v>
+      </c>
+      <c r="B20" t="s">
+        <v>396</v>
+      </c>
+      <c r="C20" t="s">
         <v>397</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>398</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>399</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>400</v>
-      </c>
-      <c r="E20" t="s">
-        <v>401</v>
-      </c>
-      <c r="F20" t="s">
-        <v>402</v>
       </c>
       <c r="G20" t="s">
         <v>87</v>
       </c>
       <c r="H20" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J20" t="s">
         <v>79</v>
       </c>
       <c r="K20" t="s">
+        <v>402</v>
+      </c>
+      <c r="L20" t="s">
+        <v>129</v>
+      </c>
+      <c r="M20" t="s">
+        <v>403</v>
+      </c>
+      <c r="N20" t="s">
         <v>404</v>
       </c>
-      <c r="L20" t="s">
-        <v>130</v>
-      </c>
-      <c r="M20" t="s">
+      <c r="O20" t="s">
         <v>405</v>
-      </c>
-      <c r="N20" t="s">
-        <v>406</v>
-      </c>
-      <c r="O20" t="s">
-        <v>407</v>
       </c>
       <c r="P20" t="s">
         <v>97</v>
       </c>
       <c r="Q20" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="R20" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="S20" t="s">
         <v>35</v>
       </c>
       <c r="T20" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="U20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="V20" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="W20" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="X20" t="s">
         <v>87</v>
@@ -4287,81 +4289,81 @@
         <v>86</v>
       </c>
       <c r="Z20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA20" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="AB20" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="AC20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AD20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AE20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C21" t="s">
         <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E21" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G21" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H21" t="s">
         <v>101</v>
       </c>
       <c r="I21" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J21" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="K21" t="s">
         <v>79</v>
       </c>
       <c r="L21" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M21" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="N21" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="O21" t="s">
         <v>84</v>
       </c>
       <c r="P21" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="Q21" t="s">
         <v>43</v>
       </c>
       <c r="R21" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="S21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T21" t="s">
         <v>36</v>
@@ -4370,78 +4372,78 @@
         <v>43</v>
       </c>
       <c r="V21" t="s">
+        <v>418</v>
+      </c>
+      <c r="W21" t="s">
+        <v>419</v>
+      </c>
+      <c r="X21" t="s">
         <v>420</v>
       </c>
-      <c r="W21" t="s">
+      <c r="Y21" t="s">
+        <v>252</v>
+      </c>
+      <c r="Z21" t="s">
         <v>421</v>
       </c>
-      <c r="X21" t="s">
+      <c r="AA21" t="s">
         <v>422</v>
       </c>
-      <c r="Y21" t="s">
-        <v>253</v>
-      </c>
-      <c r="Z21" t="s">
+      <c r="AB21" t="s">
         <v>423</v>
       </c>
-      <c r="AA21" t="s">
+      <c r="AC21" t="s">
         <v>424</v>
       </c>
-      <c r="AB21" t="s">
-        <v>425</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>426</v>
-      </c>
       <c r="AD21" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="AE21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>425</v>
+      </c>
+      <c r="B22" t="s">
+        <v>217</v>
+      </c>
+      <c r="C22" t="s">
+        <v>426</v>
+      </c>
+      <c r="D22" t="s">
+        <v>417</v>
+      </c>
+      <c r="E22" t="s">
+        <v>233</v>
+      </c>
+      <c r="F22" t="s">
+        <v>212</v>
+      </c>
+      <c r="G22" t="s">
         <v>427</v>
       </c>
-      <c r="B22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="H22" t="s">
         <v>428</v>
       </c>
-      <c r="D22" t="s">
-        <v>419</v>
-      </c>
-      <c r="E22" t="s">
-        <v>234</v>
-      </c>
-      <c r="F22" t="s">
-        <v>213</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>429</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>430</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>431</v>
       </c>
-      <c r="J22" t="s">
+      <c r="L22" t="s">
+        <v>156</v>
+      </c>
+      <c r="M22" t="s">
         <v>432</v>
       </c>
-      <c r="K22" t="s">
-        <v>433</v>
-      </c>
-      <c r="L22" t="s">
-        <v>157</v>
-      </c>
-      <c r="M22" t="s">
-        <v>434</v>
-      </c>
       <c r="N22" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="O22" t="s">
         <v>72</v>
@@ -4450,49 +4452,49 @@
         <v>72</v>
       </c>
       <c r="Q22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R22" t="s">
         <v>43</v>
       </c>
       <c r="S22" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="T22" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="U22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V22" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="W22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="X22" t="s">
         <v>38</v>
       </c>
       <c r="Y22" t="s">
+        <v>435</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>436</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB22" t="s">
         <v>437</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>438</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>439</v>
       </c>
       <c r="AC22" t="s">
         <v>41</v>
       </c>
       <c r="AD22" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="AE22" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -4500,19 +4502,19 @@
         <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C23" t="s">
+        <v>439</v>
+      </c>
+      <c r="D23" t="s">
+        <v>440</v>
+      </c>
+      <c r="E23" t="s">
+        <v>279</v>
+      </c>
+      <c r="F23" t="s">
         <v>441</v>
-      </c>
-      <c r="D23" t="s">
-        <v>442</v>
-      </c>
-      <c r="E23" t="s">
-        <v>280</v>
-      </c>
-      <c r="F23" t="s">
-        <v>443</v>
       </c>
       <c r="G23" t="s">
         <v>57</v>
@@ -4524,46 +4526,46 @@
         <v>51</v>
       </c>
       <c r="J23" t="s">
+        <v>442</v>
+      </c>
+      <c r="K23" t="s">
+        <v>417</v>
+      </c>
+      <c r="L23" t="s">
+        <v>139</v>
+      </c>
+      <c r="M23" t="s">
+        <v>443</v>
+      </c>
+      <c r="N23" t="s">
         <v>444</v>
       </c>
-      <c r="K23" t="s">
-        <v>419</v>
-      </c>
-      <c r="L23" t="s">
-        <v>140</v>
-      </c>
-      <c r="M23" t="s">
+      <c r="O23" t="s">
         <v>445</v>
       </c>
-      <c r="N23" t="s">
+      <c r="P23" t="s">
         <v>446</v>
-      </c>
-      <c r="O23" t="s">
-        <v>447</v>
-      </c>
-      <c r="P23" t="s">
-        <v>448</v>
       </c>
       <c r="Q23" t="s">
         <v>72</v>
       </c>
       <c r="R23" t="s">
+        <v>447</v>
+      </c>
+      <c r="S23" t="s">
+        <v>448</v>
+      </c>
+      <c r="T23" t="s">
         <v>449</v>
       </c>
-      <c r="S23" t="s">
-        <v>450</v>
-      </c>
-      <c r="T23" t="s">
-        <v>451</v>
-      </c>
       <c r="U23" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="V23" t="s">
         <v>93</v>
       </c>
       <c r="W23" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="X23" t="s">
         <v>57</v>
@@ -4572,114 +4574,114 @@
         <v>83</v>
       </c>
       <c r="Z23" t="s">
+        <v>451</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>378</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC23" t="s">
         <v>453</v>
       </c>
-      <c r="AA23" t="s">
-        <v>380</v>
-      </c>
-      <c r="AB23" t="s">
+      <c r="AD23" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE23" t="s">
         <v>454</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>158</v>
-      </c>
-      <c r="AE23" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B24" t="s">
         <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D24" t="s">
         <v>86</v>
       </c>
       <c r="E24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G24" t="s">
+        <v>456</v>
+      </c>
+      <c r="H24" t="s">
+        <v>457</v>
+      </c>
+      <c r="I24" t="s">
         <v>458</v>
-      </c>
-      <c r="H24" t="s">
-        <v>459</v>
-      </c>
-      <c r="I24" t="s">
-        <v>460</v>
       </c>
       <c r="J24" t="s">
         <v>73</v>
       </c>
       <c r="K24" t="s">
+        <v>459</v>
+      </c>
+      <c r="L24" t="s">
+        <v>460</v>
+      </c>
+      <c r="M24" t="s">
+        <v>382</v>
+      </c>
+      <c r="N24" t="s">
+        <v>115</v>
+      </c>
+      <c r="O24" t="s">
         <v>461</v>
       </c>
-      <c r="L24" t="s">
-        <v>462</v>
-      </c>
-      <c r="M24" t="s">
-        <v>384</v>
-      </c>
-      <c r="N24" t="s">
-        <v>116</v>
-      </c>
-      <c r="O24" t="s">
-        <v>463</v>
-      </c>
       <c r="P24" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="Q24" t="s">
         <v>38</v>
       </c>
       <c r="R24" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="S24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="T24" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="U24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V24" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="W24" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="X24" t="s">
         <v>111</v>
       </c>
       <c r="Y24" t="s">
+        <v>464</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>361</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>465</v>
+      </c>
+      <c r="AB24" t="s">
         <v>466</v>
       </c>
-      <c r="Z24" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA24" t="s">
+      <c r="AC24" t="s">
         <v>467</v>
       </c>
-      <c r="AB24" t="s">
+      <c r="AD24" t="s">
         <v>468</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>470</v>
       </c>
       <c r="AE24" t="s">
         <v>65</v>
@@ -4690,7 +4692,7 @@
         <v>104</v>
       </c>
       <c r="B25" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C25" t="s">
         <v>47</v>
@@ -4699,58 +4701,58 @@
         <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F25" t="s">
+        <v>470</v>
+      </c>
+      <c r="G25" t="s">
+        <v>471</v>
+      </c>
+      <c r="H25" t="s">
         <v>472</v>
-      </c>
-      <c r="G25" t="s">
-        <v>473</v>
-      </c>
-      <c r="H25" t="s">
-        <v>474</v>
       </c>
       <c r="I25" t="s">
         <v>48</v>
       </c>
       <c r="J25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M25" t="s">
         <v>93</v>
       </c>
       <c r="N25" t="s">
+        <v>474</v>
+      </c>
+      <c r="O25" t="s">
+        <v>475</v>
+      </c>
+      <c r="P25" t="s">
         <v>476</v>
-      </c>
-      <c r="O25" t="s">
-        <v>477</v>
-      </c>
-      <c r="P25" t="s">
-        <v>478</v>
       </c>
       <c r="Q25" t="s">
         <v>40</v>
       </c>
       <c r="R25" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="S25" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="T25" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="U25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="V25" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="W25" t="s">
         <v>38</v>
@@ -4759,117 +4761,117 @@
         <v>113</v>
       </c>
       <c r="Y25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z25" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="AA25" t="s">
         <v>36</v>
       </c>
       <c r="AB25" t="s">
+        <v>478</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>479</v>
+      </c>
+      <c r="AE25" t="s">
         <v>480</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>129</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>481</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C26" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E26" t="s">
         <v>93</v>
       </c>
       <c r="F26" t="s">
+        <v>483</v>
+      </c>
+      <c r="G26" t="s">
+        <v>484</v>
+      </c>
+      <c r="H26" t="s">
+        <v>192</v>
+      </c>
+      <c r="I26" t="s">
+        <v>197</v>
+      </c>
+      <c r="J26" t="s">
         <v>485</v>
-      </c>
-      <c r="G26" t="s">
-        <v>486</v>
-      </c>
-      <c r="H26" t="s">
-        <v>193</v>
-      </c>
-      <c r="I26" t="s">
-        <v>198</v>
-      </c>
-      <c r="J26" t="s">
-        <v>487</v>
       </c>
       <c r="K26" t="s">
         <v>44</v>
       </c>
       <c r="L26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M26" t="s">
+        <v>486</v>
+      </c>
+      <c r="N26" t="s">
+        <v>487</v>
+      </c>
+      <c r="O26" t="s">
+        <v>438</v>
+      </c>
+      <c r="P26" t="s">
         <v>488</v>
       </c>
-      <c r="N26" t="s">
+      <c r="Q26" t="s">
+        <v>127</v>
+      </c>
+      <c r="R26" t="s">
+        <v>205</v>
+      </c>
+      <c r="S26" t="s">
+        <v>163</v>
+      </c>
+      <c r="T26" t="s">
         <v>489</v>
       </c>
-      <c r="O26" t="s">
-        <v>440</v>
-      </c>
-      <c r="P26" t="s">
+      <c r="U26" t="s">
         <v>490</v>
       </c>
-      <c r="Q26" t="s">
-        <v>128</v>
-      </c>
-      <c r="R26" t="s">
-        <v>206</v>
-      </c>
-      <c r="S26" t="s">
-        <v>164</v>
-      </c>
-      <c r="T26" t="s">
-        <v>491</v>
-      </c>
-      <c r="U26" t="s">
-        <v>492</v>
-      </c>
       <c r="V26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="W26" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="X26" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="Y26" t="s">
         <v>56</v>
       </c>
       <c r="Z26" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="AA26" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="AB26" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="AC26" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="AD26" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="AE26" t="s">
         <v>48</v>

</xml_diff>